<commit_message>
source code von HPES lab5 für cmd line
</commit_message>
<xml_diff>
--- a/07_Kommandozeile/Kommandozeile.xlsx
+++ b/07_Kommandozeile/Kommandozeile.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10240" yWindow="0" windowWidth="23360" windowHeight="14840"/>
+    <workbookView xWindow="1240" yWindow="0" windowWidth="20860" windowHeight="15560"/>
   </bookViews>
   <sheets>
     <sheet name="Kommandozeile" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
   <si>
     <t>Kommandos</t>
   </si>
@@ -31,33 +31,18 @@
     <t>Argumente</t>
   </si>
   <si>
-    <t>Sensoridentifizierung</t>
-  </si>
-  <si>
     <t>Messsmodus</t>
   </si>
   <si>
-    <t>Timestamp sync</t>
-  </si>
-  <si>
     <t>Zeige Verzeichnis</t>
   </si>
   <si>
-    <t>Messparameter einstellen (alle oder einzeln)</t>
-  </si>
-  <si>
     <t>CAN-Priorität setzen (Menügeführt)</t>
   </si>
   <si>
     <t>Sensorstatus (Messparameter, Cachefüllstand, CAN-Errors?)</t>
   </si>
   <si>
-    <t>Schliesse Files</t>
-  </si>
-  <si>
-    <t>Karte unmount</t>
-  </si>
-  <si>
     <t>Karte mount</t>
   </si>
   <si>
@@ -65,6 +50,106 @@
   </si>
   <si>
     <t>file löschen</t>
+  </si>
+  <si>
+    <t>mode</t>
+  </si>
+  <si>
+    <t>1..4</t>
+  </si>
+  <si>
+    <t>ls</t>
+  </si>
+  <si>
+    <t>[-a] 1..</t>
+  </si>
+  <si>
+    <t>Loggerstatus (Samplingrate, Speicherplatz SD, Speicherplatz RAM, alle Sensoren sichtbar?...)</t>
+  </si>
+  <si>
+    <t>sd_mount</t>
+  </si>
+  <si>
+    <t>sd_unmount</t>
+  </si>
+  <si>
+    <t>sd_format</t>
+  </si>
+  <si>
+    <t>rm</t>
+  </si>
+  <si>
+    <t>time</t>
+  </si>
+  <si>
+    <t>-s</t>
+  </si>
+  <si>
+    <t>interne Uhrzeit anzeigen, -s setzt die Uhrzeit (jjjj mm tt hh mm ss)</t>
+  </si>
+  <si>
+    <t>sensor_priority</t>
+  </si>
+  <si>
+    <t>sensor_state</t>
+  </si>
+  <si>
+    <t>logger_state</t>
+  </si>
+  <si>
+    <t>Messparameter einstellen (nur alle oder auch einzeln?)</t>
+  </si>
+  <si>
+    <t>1) find sensors</t>
+  </si>
+  <si>
+    <t>2) rearrange priority</t>
+  </si>
+  <si>
+    <t>listet die sensoren auf, sie können umsortiert werden</t>
+  </si>
+  <si>
+    <t>sensor_parameters</t>
+  </si>
+  <si>
+    <t>Kategorie</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>setup</t>
+  </si>
+  <si>
+    <t>Karte unmount, Schliesse Files</t>
+  </si>
+  <si>
+    <t>logging</t>
+  </si>
+  <si>
+    <t>start/stop</t>
+  </si>
+  <si>
+    <t>stoppen vor dem unmounten, starten nach dem mounten</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>timestamp</t>
+  </si>
+  <si>
+    <t>Timestamp anzeigen, -s synchronisiert alle Sensoren</t>
+  </si>
+  <si>
+    <t>Erkärung</t>
+  </si>
+  <si>
+    <t>Output</t>
+  </si>
+  <si>
+    <t>Timestamp wird ausgegeben.
+Beim synchronisieren wird erst eine Meldung ausgegeben, danach alle Sensoren synchronisiert. Nach erfolgreichem sync wird eine Erfolgsmeldung ausgegeben.</t>
   </si>
 </sst>
 </file>
@@ -117,7 +202,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -125,23 +210,61 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -441,86 +564,226 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="4" max="4" width="47.6640625" customWidth="1"/>
+    <col min="5" max="5" width="29.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="C3" t="s">
+      <c r="C2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="4"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="C5" t="s">
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="4"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="C7" t="s">
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="7"/>
+      <c r="C11" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="4"/>
+      <c r="C12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="C8" t="s">
+      <c r="E12" s="4"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="C10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="C11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="C12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="C13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="C14" t="s">
-        <v>14</v>
-      </c>
+      <c r="E13" s="4"/>
+    </row>
+    <row r="14" spans="1:5" ht="84">
+      <c r="A14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="4"/>
     </row>
   </sheetData>
+  <sortState ref="A3:D14">
+    <sortCondition ref="C3:C14"/>
+    <sortCondition ref="A3:A14"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
   <extLst>
@@ -533,31 +796,39 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
     <col min="3" max="3" width="101.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="2"/>
-      <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
+      <c r="A2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
+      <c r="B3" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="3"/>
@@ -626,17 +897,17 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
+      <c r="B17" s="3"/>
       <c r="C17" s="2"/>
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
+      <c r="B18" s="2"/>
       <c r="C18" s="3"/>
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
+      <c r="B19" s="3"/>
       <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:3">
@@ -679,8 +950,12 @@
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
     </row>
+    <row r="28" spans="1:3">
+      <c r="B28" s="2"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Kommandozeile neu angefangen, dafür läuft es schon fast fast
</commit_message>
<xml_diff>
--- a/07_Kommandozeile/Kommandozeile.xlsx
+++ b/07_Kommandozeile/Kommandozeile.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
-  <workbookPr autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="14720" yWindow="0" windowWidth="20860" windowHeight="15560"/>
+    <workbookView xWindow="14715" yWindow="0" windowWidth="20865" windowHeight="15555"/>
   </bookViews>
   <sheets>
     <sheet name="Kommandozeile" sheetId="1" r:id="rId1"/>
     <sheet name="Menüstruktur" sheetId="2" r:id="rId2"/>
+    <sheet name="Tabelle1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="77">
   <si>
     <t>Kommandos</t>
   </si>
@@ -164,6 +165,96 @@
   </si>
   <si>
     <t>Timestamp anzeigen, -s synchronisiert alle Sensoren, -c vergleicht die Timestamps aller Sensoreinheiten</t>
+  </si>
+  <si>
+    <t>cmd_list</t>
+  </si>
+  <si>
+    <t>list files</t>
+  </si>
+  <si>
+    <t>format sd card</t>
+  </si>
+  <si>
+    <t>mount sd card</t>
+  </si>
+  <si>
+    <t>unmount sd card</t>
+  </si>
+  <si>
+    <t>logger status</t>
+  </si>
+  <si>
+    <t>start/stop logging</t>
+  </si>
+  <si>
+    <t>detail level</t>
+  </si>
+  <si>
+    <t>sensor parameters</t>
+  </si>
+  <si>
+    <t>sensor state</t>
+  </si>
+  <si>
+    <t>reset timestamp</t>
+  </si>
+  <si>
+    <t>internal clock</t>
+  </si>
+  <si>
+    <t>##</t>
+  </si>
+  <si>
+    <t>delete file no.</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>exit</t>
+  </si>
+  <si>
+    <t>raw</t>
+  </si>
+  <si>
+    <t>detailed</t>
+  </si>
+  <si>
+    <t>peaks only</t>
+  </si>
+  <si>
+    <t>sparse</t>
+  </si>
+  <si>
+    <t>sampling rate</t>
+  </si>
+  <si>
+    <t>threshold</t>
+  </si>
+  <si>
+    <t>base line value</t>
+  </si>
+  <si>
+    <t>timeout</t>
+  </si>
+  <si>
+    <t>reset</t>
+  </si>
+  <si>
+    <t>set clock</t>
+  </si>
+  <si>
+    <t>(not a state because we only show the result of the try)</t>
+  </si>
+  <si>
+    <t>(not a state because we only display the state)</t>
+  </si>
+  <si>
+    <t>==&gt; ask for number of sensor(maybe ad option for ALL)</t>
   </si>
 </sst>
 </file>
@@ -208,12 +299,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -243,7 +346,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -274,15 +377,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -584,21 +696,22 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD15"/>
+      <selection activeCell="A13" sqref="A13:D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="47.6640625" customWidth="1"/>
-    <col min="5" max="5" width="29.1640625" customWidth="1"/>
+    <col min="1" max="1" width="22.85546875" customWidth="1"/>
+    <col min="4" max="4" width="47.7109375" customWidth="1"/>
+    <col min="5" max="5" width="29.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -615,7 +728,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>12</v>
       </c>
@@ -628,7 +741,7 @@
       </c>
       <c r="E3" s="4"/>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>18</v>
       </c>
@@ -641,7 +754,7 @@
       </c>
       <c r="E4" s="4"/>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
@@ -654,7 +767,7 @@
       </c>
       <c r="E5" s="4"/>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>15</v>
       </c>
@@ -667,7 +780,7 @@
       </c>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>16</v>
       </c>
@@ -680,7 +793,7 @@
       </c>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>24</v>
       </c>
@@ -693,7 +806,7 @@
       </c>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>34</v>
       </c>
@@ -708,7 +821,7 @@
       </c>
       <c r="E9" s="4"/>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>10</v>
       </c>
@@ -723,7 +836,7 @@
       </c>
       <c r="E10" s="4"/>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>29</v>
       </c>
@@ -736,7 +849,7 @@
       </c>
       <c r="E11" s="4"/>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>22</v>
       </c>
@@ -749,22 +862,22 @@
       </c>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="C13" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="15" t="s">
         <v>6</v>
       </c>
       <c r="E13" s="4"/>
     </row>
-    <row r="14" spans="1:5" ht="84">
+    <row r="14" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>38</v>
       </c>
@@ -781,7 +894,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>19</v>
       </c>
@@ -796,7 +909,7 @@
       </c>
       <c r="E15" s="4"/>
     </row>
-    <row r="16" spans="1:5" ht="70">
+    <row r="16" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
         <v>42</v>
       </c>
@@ -833,17 +946,17 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="101.1640625" customWidth="1"/>
+    <col min="3" max="3" width="101.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>22</v>
       </c>
@@ -852,7 +965,7 @@
       </c>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="3"/>
       <c r="B3" s="2" t="s">
         <v>27</v>
@@ -861,127 +974,127 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
       <c r="B10" s="3"/>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
       <c r="B12" s="3"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
       <c r="B17" s="3"/>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3"/>
       <c r="B18" s="2"/>
       <c r="C18" s="3"/>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
       <c r="B19" s="3"/>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
     </row>
   </sheetData>
@@ -993,4 +1106,320 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E45"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26:D30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>5</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C14" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>7</v>
+      </c>
+      <c r="B19" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>8</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>2</v>
+      </c>
+      <c r="D27" s="12" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>3</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <v>4</v>
+      </c>
+      <c r="D29" s="12" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>5</v>
+      </c>
+      <c r="D30" s="12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D32">
+        <v>2</v>
+      </c>
+      <c r="E32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D33">
+        <v>3</v>
+      </c>
+      <c r="E33" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D34">
+        <v>4</v>
+      </c>
+      <c r="E34" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>9</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>10</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>11</v>
+      </c>
+      <c r="B43" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>